<commit_message>
added some pictures and fix a Date bug
</commit_message>
<xml_diff>
--- a/Planing.xlsx
+++ b/Planing.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p253237\PhpstormProjects\Advent\Advent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapha\PhpstormProjects\Advent\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD1993F-4559-408D-9298-E76702F590D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>Datum</t>
   </si>
@@ -153,12 +145,15 @@
   </si>
   <si>
     <t>you generace</t>
+  </si>
+  <si>
+    <t>No pic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -540,11 +535,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +548,7 @@
     <col min="3" max="3" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,7 +559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44531</v>
       </c>
@@ -575,7 +570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44532</v>
       </c>
@@ -586,7 +581,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44533</v>
       </c>
@@ -596,8 +591,11 @@
       <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44534</v>
       </c>
@@ -608,7 +606,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44535</v>
       </c>
@@ -619,7 +617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44536</v>
       </c>
@@ -630,7 +628,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44537</v>
       </c>
@@ -640,8 +638,11 @@
       <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44538</v>
       </c>
@@ -652,7 +653,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44539</v>
       </c>
@@ -663,7 +664,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>44540</v>
       </c>
@@ -673,8 +674,11 @@
       <c r="C11" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>44541</v>
       </c>
@@ -685,7 +689,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44542</v>
       </c>
@@ -696,7 +700,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44543</v>
       </c>
@@ -707,7 +711,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44544</v>
       </c>
@@ -718,7 +722,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>44545</v>
       </c>
@@ -728,8 +732,11 @@
       <c r="C16" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>44546</v>
       </c>
@@ -740,7 +747,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>44547</v>
       </c>
@@ -751,7 +758,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44548</v>
       </c>
@@ -761,8 +768,11 @@
       <c r="C19" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44549</v>
       </c>
@@ -773,7 +783,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44550</v>
       </c>
@@ -783,16 +793,22 @@
       <c r="C21" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44551</v>
       </c>
       <c r="B22" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44552</v>
       </c>
@@ -802,8 +818,11 @@
       <c r="C23" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>44553</v>
       </c>
@@ -813,8 +832,11 @@
       <c r="C24" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>44554</v>
       </c>
@@ -824,8 +846,11 @@
       <c r="C25" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
red border for current day, added song cover for day 7 and spotify links
</commit_message>
<xml_diff>
--- a/Planing.xlsx
+++ b/Planing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapha\PhpstormProjects\Advent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD1993F-4559-408D-9298-E76702F590D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DD9653-B1D0-4A14-A2D6-BDD266F30C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>Datum</t>
   </si>
@@ -148,6 +148,15 @@
   </si>
   <si>
     <t>No pic</t>
+  </si>
+  <si>
+    <t>Crash Bendicat</t>
+  </si>
+  <si>
+    <t>Song</t>
+  </si>
+  <si>
+    <t>Berry White</t>
   </si>
 </sst>
 </file>
@@ -215,13 +224,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -539,16 +549,16 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>44531</v>
       </c>
@@ -570,7 +580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>44532</v>
       </c>
@@ -581,21 +591,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>44533</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>44534</v>
       </c>
@@ -606,7 +613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>44535</v>
       </c>
@@ -617,7 +624,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>44536</v>
       </c>
@@ -628,21 +635,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>44537</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>8</v>
+      <c r="B8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="D8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>44538</v>
       </c>
@@ -653,7 +660,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>44539</v>
       </c>
@@ -664,7 +671,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>44540</v>
       </c>
@@ -678,7 +685,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>44541</v>
       </c>
@@ -689,7 +696,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>44542</v>
       </c>
@@ -700,7 +707,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>44543</v>
       </c>
@@ -711,7 +718,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>44544</v>
       </c>
@@ -722,7 +729,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>44545</v>
       </c>
@@ -736,7 +743,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>44546</v>
       </c>
@@ -747,7 +754,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>44547</v>
       </c>
@@ -758,7 +765,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>44548</v>
       </c>
@@ -772,7 +779,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>44549</v>
       </c>
@@ -783,7 +790,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>44550</v>
       </c>
@@ -797,7 +804,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>44551</v>
       </c>
@@ -808,7 +815,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>44552</v>
       </c>
@@ -822,7 +829,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>44553</v>
       </c>
@@ -836,7 +843,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>44554</v>
       </c>
@@ -850,7 +857,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:4" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added content + photos
</commit_message>
<xml_diff>
--- a/Planing.xlsx
+++ b/Planing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapha\PhpstormProjects\Advent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DD9653-B1D0-4A14-A2D6-BDD266F30C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA09C76B-6785-4523-8821-41177E22E3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>Datum</t>
   </si>
@@ -157,6 +157,15 @@
   </si>
   <si>
     <t>Berry White</t>
+  </si>
+  <si>
+    <t>Ill never do you wrong</t>
+  </si>
+  <si>
+    <t>HelpingHand</t>
+  </si>
+  <si>
+    <t>It rains love</t>
   </si>
 </sst>
 </file>
@@ -548,17 +557,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -569,7 +578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44531</v>
       </c>
@@ -580,7 +589,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44532</v>
       </c>
@@ -591,7 +600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44533</v>
       </c>
@@ -602,7 +611,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44534</v>
       </c>
@@ -613,7 +622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44535</v>
       </c>
@@ -624,7 +633,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44536</v>
       </c>
@@ -635,7 +644,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44537</v>
       </c>
@@ -645,11 +654,8 @@
       <c r="C8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44538</v>
       </c>
@@ -660,7 +666,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44539</v>
       </c>
@@ -671,21 +677,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>44540</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>44541</v>
       </c>
@@ -696,7 +699,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44542</v>
       </c>
@@ -707,7 +710,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44543</v>
       </c>
@@ -718,7 +721,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44544</v>
       </c>
@@ -729,21 +732,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>44545</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>44546</v>
       </c>
@@ -754,7 +754,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>44547</v>
       </c>
@@ -765,21 +765,19 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44548</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44549</v>
       </c>
@@ -790,7 +788,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44550</v>
       </c>
@@ -800,22 +798,16 @@
       <c r="C21" t="s">
         <v>34</v>
       </c>
-      <c r="D21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44551</v>
       </c>
       <c r="B22" t="s">
         <v>37</v>
       </c>
-      <c r="D22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44552</v>
       </c>
@@ -825,11 +817,8 @@
       <c r="C23" t="s">
         <v>36</v>
       </c>
-      <c r="D23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>44553</v>
       </c>
@@ -843,7 +832,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>44554</v>
       </c>
@@ -857,7 +846,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:4" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
finished stuff to give
</commit_message>
<xml_diff>
--- a/Planing.xlsx
+++ b/Planing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p253237\WebstormProjects\Advent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A641796-97F1-4FA5-9D13-06F60001DBCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C7D054-35D5-469F-9C2D-77465CE934BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Datum</t>
   </si>
@@ -36,12 +36,6 @@
     <t>Beschreibung</t>
   </si>
   <si>
-    <t>Sweets</t>
-  </si>
-  <si>
-    <t>Sweets for my sweety</t>
-  </si>
-  <si>
     <t>Haarbändeli</t>
   </si>
   <si>
@@ -54,9 +48,6 @@
     <t>Text</t>
   </si>
   <si>
-    <t>Big Present</t>
-  </si>
-  <si>
     <t>IDK</t>
   </si>
   <si>
@@ -90,28 +81,55 @@
     <t>cause u need one</t>
   </si>
   <si>
-    <t>t-shirt</t>
-  </si>
-  <si>
-    <t>table for two</t>
-  </si>
-  <si>
-    <t>table for two at Circolo Popolare</t>
-  </si>
-  <si>
-    <t>you generace</t>
-  </si>
-  <si>
     <t>No pic</t>
   </si>
   <si>
     <t>Song</t>
   </si>
   <si>
-    <t>merch?</t>
-  </si>
-  <si>
-    <t>traveling thingy?</t>
+    <t>Vegan Schoki</t>
+  </si>
+  <si>
+    <t>ducky</t>
+  </si>
+  <si>
+    <t>duck on the tv</t>
+  </si>
+  <si>
+    <t>drink</t>
+  </si>
+  <si>
+    <t>schmuck</t>
+  </si>
+  <si>
+    <t>restaurant reservations</t>
+  </si>
+  <si>
+    <t>fcz schal</t>
+  </si>
+  <si>
+    <t>fcz stuff</t>
+  </si>
+  <si>
+    <t>schoki</t>
+  </si>
+  <si>
+    <t>salty snack</t>
+  </si>
+  <si>
+    <t>stampfer</t>
+  </si>
+  <si>
+    <t>spende</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vegan Schoki </t>
+  </si>
+  <si>
+    <t>Little Simz</t>
+  </si>
+  <si>
+    <t>Christmas Song</t>
   </si>
 </sst>
 </file>
@@ -156,7 +174,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -184,7 +202,15 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -497,7 +523,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,10 +548,10 @@
         <v>44531</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -533,10 +559,10 @@
         <v>44532</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -544,7 +570,7 @@
         <v>44533</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -552,21 +578,27 @@
       <c r="A5" s="2">
         <v>44534</v>
       </c>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44535</v>
       </c>
+      <c r="B6" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44536</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -574,19 +606,21 @@
         <v>44537</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44538</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -594,7 +628,7 @@
         <v>44539</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -602,7 +636,7 @@
         <v>44540</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C11" s="4"/>
     </row>
@@ -611,26 +645,32 @@
         <v>44541</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44542</v>
       </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44543</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -638,10 +678,7 @@
         <v>44544</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -649,7 +686,7 @@
         <v>44545</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C16" s="4"/>
     </row>
@@ -657,16 +694,19 @@
       <c r="A17" s="2">
         <v>44546</v>
       </c>
+      <c r="B17" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44547</v>
       </c>
       <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
         <v>27</v>
-      </c>
-      <c r="C18" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -674,7 +714,7 @@
         <v>44548</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -683,8 +723,8 @@
       <c r="A20" s="2">
         <v>44549</v>
       </c>
-      <c r="C20" t="s">
-        <v>24</v>
+      <c r="B20" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -692,31 +732,40 @@
         <v>44550</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44551</v>
       </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44552</v>
       </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44553</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -724,17 +773,22 @@
         <v>44554</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Song">
+      <formula>NOT(ISERROR(SEARCH("Song",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>